<commit_message>
Create separate sheets with cost/weights
</commit_message>
<xml_diff>
--- a/RoundTube_Export.xlsx
+++ b/RoundTube_Export.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schimmer\OneDrive - Rose-Hulman Institute of Technology\Documents\!! RHIT Fall 2021-22\EM204\EM204_Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E3B71B-96BF-4EB7-85D6-85DA01AB1EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDD5EFE-7741-4767-B3DD-F1EC84104EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14985" yWindow="1920" windowWidth="13500" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14985" yWindow="1995" windowWidth="13500" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$37</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,41 +33,10 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>OD</t>
-  </si>
-  <si>
-    <t>Wall</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Shear Stress [ksi]</t>
-  </si>
-  <si>
-    <t>Cost [$]</t>
-  </si>
-  <si>
-    <t>Weight [lb/ft]</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -100,7 +66,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,400 +381,385 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63F18A3-AA89-4C27-A2B8-63FBF8EF687B}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>4.5</v>
+      </c>
+      <c r="B1">
+        <v>0.125</v>
+      </c>
+      <c r="C1">
+        <v>4.25</v>
+      </c>
+      <c r="D1">
+        <v>6.5630439399371303</v>
+      </c>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3.25</v>
+      </c>
+      <c r="B2">
+        <v>0.25</v>
+      </c>
+      <c r="C2">
+        <v>2.75</v>
+      </c>
+      <c r="D2">
+        <v>7.3057606980665888</v>
+      </c>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>0.75</v>
-      </c>
-      <c r="C2">
-        <v>1.5</v>
-      </c>
-      <c r="D2">
-        <v>4.8288788659585435</v>
-      </c>
-      <c r="E2">
-        <v>6.24</v>
-      </c>
-      <c r="F2">
-        <v>389.32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
       <c r="B3">
-        <v>0.375</v>
+        <v>0.125</v>
       </c>
       <c r="C3">
-        <v>2.25</v>
+        <v>4.75</v>
       </c>
       <c r="D3">
-        <v>6.6224624447431442</v>
-      </c>
-      <c r="E3">
-        <v>3.64</v>
-      </c>
-      <c r="F3">
-        <v>394.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5.2715952443497693</v>
+      </c>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="B4">
         <v>0.25</v>
       </c>
       <c r="C4">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>7.3057606980665888</v>
-      </c>
-      <c r="E4">
-        <v>2.78</v>
-      </c>
-      <c r="F4">
-        <v>236.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6.1945120294083571</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="C5">
+        <v>5.75</v>
+      </c>
+      <c r="D5">
+        <v>3.6150343758249384</v>
+      </c>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.1875</v>
+      </c>
+      <c r="C6">
+        <v>3.625</v>
+      </c>
+      <c r="D6">
+        <v>5.8677467976100646</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.1875</v>
+      </c>
+      <c r="C7">
+        <v>4.625</v>
+      </c>
+      <c r="D7">
+        <v>3.6499685846283296</v>
+      </c>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>3</v>
       </c>
-      <c r="D5">
-        <v>6.1945120294083571</v>
-      </c>
-      <c r="E5">
-        <v>3.01</v>
-      </c>
-      <c r="F5">
-        <v>338.87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3.5</v>
-      </c>
-      <c r="B6">
-        <v>0.5</v>
-      </c>
-      <c r="C6">
-        <v>2.5</v>
-      </c>
-      <c r="D6">
-        <v>3.8541305137929247</v>
-      </c>
-      <c r="E6">
-        <v>5.71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3.5</v>
-      </c>
-      <c r="B7">
+      <c r="B8">
         <v>0.375</v>
       </c>
-      <c r="C7">
-        <v>2.75</v>
-      </c>
-      <c r="D7">
-        <v>4.6064762431099791</v>
-      </c>
-      <c r="E7">
-        <v>4.47</v>
-      </c>
-      <c r="F7">
-        <v>618.46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>0.1875</v>
-      </c>
       <c r="C8">
-        <v>3.625</v>
+        <v>2.25</v>
       </c>
       <c r="D8">
-        <v>5.8677467976100646</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6.6224624447431442</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="C9">
-        <v>3.5</v>
+        <v>6.75</v>
       </c>
       <c r="D9">
-        <v>4.6152116595002006</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.6321930584615698</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
       <c r="B10">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D10">
-        <v>2.7938513438760144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4.6152116595002006</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4.25</v>
+        <v>4.5</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="C11">
-        <v>3.25</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>2.4197111347980038</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.5702359972452107</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>4.5</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>0.125</v>
       </c>
       <c r="C12">
-        <v>4.25</v>
+        <v>7.75</v>
       </c>
       <c r="D12">
-        <v>6.5630439399371303</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.0017518724664418</v>
+      </c>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="B13">
         <v>0.25</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="D13">
-        <v>3.5702359972452107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.8434078812346759</v>
+      </c>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>0.75</v>
+      </c>
+      <c r="C14">
+        <v>1.5</v>
+      </c>
+      <c r="D14">
+        <v>4.8288788659585435</v>
+      </c>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3.5</v>
+      </c>
+      <c r="B15">
+        <v>0.375</v>
+      </c>
+      <c r="C15">
+        <v>2.75</v>
+      </c>
+      <c r="D15">
+        <v>4.6064762431099791</v>
+      </c>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>0.1875</v>
+      </c>
+      <c r="C16">
+        <v>5.625</v>
+      </c>
+      <c r="D16">
+        <v>2.4871430280035951</v>
+      </c>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>4.5</v>
       </c>
-      <c r="B14">
+      <c r="B17">
         <v>0.375</v>
       </c>
-      <c r="C14">
+      <c r="C17">
         <v>3.75</v>
       </c>
-      <c r="D14">
+      <c r="D17">
         <v>2.5907546821834209</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>4.5</v>
-      </c>
-      <c r="B15">
-        <v>0.5</v>
-      </c>
-      <c r="C15">
-        <v>3.5</v>
-      </c>
-      <c r="D15">
-        <v>2.1155364743291938</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>4.5</v>
-      </c>
-      <c r="B16">
-        <v>0.75</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>1.6715349920625728</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>5</v>
-      </c>
-      <c r="B17">
-        <v>0.125</v>
-      </c>
-      <c r="C17">
-        <v>4.75</v>
-      </c>
-      <c r="D17">
-        <v>5.2715952443497693</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18">
-        <v>0.1875</v>
+        <v>0.25</v>
       </c>
       <c r="C18">
-        <v>4.625</v>
+        <v>5.5</v>
       </c>
       <c r="D18">
-        <v>3.6499685846283296</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.9252133952878194</v>
+      </c>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="B19">
         <v>0.25</v>
       </c>
       <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>2.3176745688262561</v>
+      </c>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3.5</v>
+      </c>
+      <c r="B20">
+        <v>0.5</v>
+      </c>
+      <c r="C20">
+        <v>2.5</v>
+      </c>
+      <c r="D20">
+        <v>3.8541305137929247</v>
+      </c>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>0.5</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>2.7938513438760144</v>
+      </c>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>0.25</v>
+      </c>
+      <c r="C22">
+        <v>7.5</v>
+      </c>
+      <c r="D22">
+        <v>1.0492634649390169</v>
+      </c>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>4.5</v>
       </c>
-      <c r="D19">
-        <v>2.8434078812346759</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="B23">
+        <v>0.5</v>
+      </c>
+      <c r="C23">
+        <v>3.5</v>
+      </c>
+      <c r="D23">
+        <v>2.1155364743291938</v>
+      </c>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>5</v>
       </c>
-      <c r="B20">
-        <v>0.5</v>
-      </c>
-      <c r="C20">
+      <c r="B24">
+        <v>0.5</v>
+      </c>
+      <c r="C24">
         <v>4</v>
       </c>
-      <c r="D20">
+      <c r="D24">
         <v>1.6562465622571223</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>5.5</v>
-      </c>
-      <c r="B21">
-        <v>0.25</v>
-      </c>
-      <c r="C21">
-        <v>5</v>
-      </c>
-      <c r="D21">
-        <v>2.3176745688262561</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>6</v>
-      </c>
-      <c r="B22">
-        <v>0.125</v>
-      </c>
-      <c r="C22">
-        <v>5.75</v>
-      </c>
-      <c r="D22">
-        <v>3.6150343758249384</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>6</v>
-      </c>
-      <c r="B23">
-        <v>0.25</v>
-      </c>
-      <c r="C23">
-        <v>5.5</v>
-      </c>
-      <c r="D23">
-        <v>1.9252133952878194</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>6</v>
-      </c>
-      <c r="B24">
-        <v>0.1875</v>
-      </c>
-      <c r="C24">
-        <v>5.625</v>
-      </c>
-      <c r="D24">
-        <v>2.4871430280035951</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -821,22 +772,24 @@
       <c r="D25">
         <v>1.0929746315461308</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="B26">
-        <v>0.125</v>
+        <v>0.75</v>
       </c>
       <c r="C26">
-        <v>6.75</v>
+        <v>3</v>
       </c>
       <c r="D26">
-        <v>2.6321930584615698</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.6715349920625728</v>
+      </c>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7</v>
       </c>
@@ -849,8 +802,9 @@
       <c r="D27">
         <v>1.3891295367825947</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7</v>
       </c>
@@ -864,74 +818,74 @@
         <v>0.77431400367604464</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>0.5</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>0.57690145743752508</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>7.5</v>
       </c>
-      <c r="B29">
-        <v>0.5</v>
-      </c>
-      <c r="C29">
+      <c r="B30">
+        <v>0.5</v>
+      </c>
+      <c r="C30">
         <v>6.5</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>0.6647806179908029</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <v>0.5</v>
+      </c>
+      <c r="C31">
         <v>8</v>
       </c>
-      <c r="B30">
-        <v>0.125</v>
-      </c>
-      <c r="C30">
-        <v>7.75</v>
-      </c>
-      <c r="D30">
-        <v>2.0017518724664418</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>8</v>
-      </c>
-      <c r="B31">
-        <v>0.25</v>
-      </c>
-      <c r="C31">
-        <v>7.5</v>
-      </c>
       <c r="D31">
-        <v>1.0492634649390169</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.44627949965565133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>8</v>
+        <v>4.25</v>
       </c>
       <c r="B32">
         <v>0.5</v>
       </c>
       <c r="C32">
-        <v>7</v>
+        <v>3.25</v>
       </c>
       <c r="D32">
-        <v>0.57690145743752508</v>
+        <v>2.4197111347980038</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B33">
-        <v>1.5</v>
+        <v>0.25</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>11.5</v>
       </c>
       <c r="D33">
-        <v>0.2817193806847032</v>
+        <v>0.4518792969781173</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -953,49 +907,30 @@
         <v>9</v>
       </c>
       <c r="B35">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D35">
-        <v>0.44627949965565133</v>
+        <v>0.26444205929114922</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C36">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D36">
-        <v>0.26444205929114922</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>12</v>
-      </c>
-      <c r="B37">
-        <v>0.25</v>
-      </c>
-      <c r="C37">
-        <v>11.5</v>
-      </c>
-      <c r="D37">
-        <v>0.4518792969781173</v>
+        <v>0.2817193806847032</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F37" xr:uid="{E63F18A3-AA89-4C27-A2B8-63FBF8EF687B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F37">
-      <sortCondition ref="A1:A37"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>